<commit_message>
webapply postman collections and scenarios file
</commit_message>
<xml_diff>
--- a/wiremock/WiremockScenarios.xlsx
+++ b/wiremock/WiremockScenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebApply\api\Guna_API\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GU287175\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
   <si>
     <t>SI No</t>
   </si>
@@ -196,6 +196,63 @@
   </si>
   <si>
     <t>BackofficeLogin</t>
+  </si>
+  <si>
+    <t>SMEProposal</t>
+  </si>
+  <si>
+    <t>COSME0007BackOfficeLoginRequest</t>
+  </si>
+  <si>
+    <t>COSME0007BackOfficeLoginResponse</t>
+  </si>
+  <si>
+    <t>COSME0008SMEProspectRequest</t>
+  </si>
+  <si>
+    <t>COSME0008SMEProspectResponse</t>
+  </si>
+  <si>
+    <t>prospectId= COSME008</t>
+  </si>
+  <si>
+    <t>UpdateSMEProposal</t>
+  </si>
+  <si>
+    <t>SearchSMEProposal</t>
+  </si>
+  <si>
+    <t>COSME0009SearchSMEProspectRequest</t>
+  </si>
+  <si>
+    <t>fname = COSME0010</t>
+  </si>
+  <si>
+    <t>COSME0010SearchSMEProspectResponse</t>
+  </si>
+  <si>
+    <t>COSME0010SearchSMEProspectRequest</t>
+  </si>
+  <si>
+    <t>Update SME Proposal</t>
+  </si>
+  <si>
+    <t>Search SME Proposal</t>
+  </si>
+  <si>
+    <t>Search Retail Proposal</t>
+  </si>
+  <si>
+    <t>Search Corporate Proposal</t>
+  </si>
+  <si>
+    <t>SearchCorporateProposal</t>
+  </si>
+  <si>
+    <t>COSME0012SearchCorporateProspectRequest</t>
+  </si>
+  <si>
+    <t>COSME0011SearchRetailProspectRequest</t>
   </si>
 </sst>
 </file>
@@ -590,19 +647,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="3" customWidth="1"/>
-    <col min="2" max="2" width="18.375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="59.875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="19.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.625" style="3" customWidth="1"/>
     <col min="6" max="6" width="29.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.5" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -779,6 +836,12 @@
       <c r="D8" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="F8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -787,6 +850,21 @@
       <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -795,6 +873,21 @@
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="C10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -803,6 +896,21 @@
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="C11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -811,6 +919,21 @@
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -818,6 +941,21 @@
       </c>
       <c r="B13" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated 2 files in wiremock
</commit_message>
<xml_diff>
--- a/wiremock/WiremockScenarios.xlsx
+++ b/wiremock/WiremockScenarios.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="104">
   <si>
     <t>SI No</t>
   </si>
@@ -253,6 +253,97 @@
   </si>
   <si>
     <t>COSME0011SearchRetailProspectRequest</t>
+  </si>
+  <si>
+    <t>COSME0013COSMECUSTOMERRequest</t>
+  </si>
+  <si>
+    <t>COSME0013SearchSMEProspectResponse</t>
+  </si>
+  <si>
+    <t>prospectId = COSME0013</t>
+  </si>
+  <si>
+    <t>prospectId = COSME0016</t>
+  </si>
+  <si>
+    <t>prospectId = COSME0019</t>
+  </si>
+  <si>
+    <t>prospectId = COSME0020</t>
+  </si>
+  <si>
+    <t>SME Customer Prospect</t>
+  </si>
+  <si>
+    <t>SME Costomer Prospects</t>
+  </si>
+  <si>
+    <t>COSME0015GetSMERequest</t>
+  </si>
+  <si>
+    <t>code = 1234</t>
+  </si>
+  <si>
+    <t>COSME0015GetSMEResponse</t>
+  </si>
+  <si>
+    <t>SME Datalist</t>
+  </si>
+  <si>
+    <t>SMEdatalist</t>
+  </si>
+  <si>
+    <t>COSME0016PostonboardSMEcustomerResponse</t>
+  </si>
+  <si>
+    <t>COSME0016PostonboardSMEcustomerRequest</t>
+  </si>
+  <si>
+    <t>OnBoardSMECustomer</t>
+  </si>
+  <si>
+    <t>COSME0017DocumentsUploadRequest</t>
+  </si>
+  <si>
+    <t>DocumentsUploadRequest</t>
+  </si>
+  <si>
+    <t>fileName = COSME0017</t>
+  </si>
+  <si>
+    <t>COSME0018GetDocumentbyidResponse</t>
+  </si>
+  <si>
+    <t>COSME0018GetDocumentbyIdRequest</t>
+  </si>
+  <si>
+    <t>prospectId =  COSME0018</t>
+  </si>
+  <si>
+    <t>GETDocumentBy ID</t>
+  </si>
+  <si>
+    <t>COSME0017DocumentsUploadResponse</t>
+  </si>
+  <si>
+    <t>COMSE0019PUTReuploadDocumentRequest</t>
+  </si>
+  <si>
+    <t>ReuploadDocument</t>
+  </si>
+  <si>
+    <t>COSME0020GETPreScreenResponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PreScreening </t>
+  </si>
+  <si>
+    <t>COSME0020GETPreScreenRequest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username = COSME0007
+  </t>
   </si>
 </sst>
 </file>
@@ -647,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -823,7 +914,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -835,6 +926,9 @@
       </c>
       <c r="D8" s="3" t="s">
         <v>54</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>56</v>
@@ -965,6 +1059,21 @@
       <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="C14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -981,48 +1090,138 @@
       <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1030,7 +1229,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>

</xml_diff>